<commit_message>
[FIX] input and output excel report form
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">รายงาน</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">ชื่อผู้ประกอบการ :</t>
   </si>
   <si>
-    <t xml:space="preserve">เลขประจำตัวผู้เสียภาษีอากร </t>
+    <t xml:space="preserve">เลขประจำตัวผู้เสียภาษีอากร</t>
   </si>
   <si>
     <t xml:space="preserve">ชื่อสถานประกอบการ :</t>
@@ -43,15 +43,12 @@
     <t xml:space="preserve">สำนักงานใหญ่</t>
   </si>
   <si>
+    <t xml:space="preserve">สาขาที่</t>
+  </si>
+  <si>
     <t xml:space="preserve">ที่อยู่ :</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">สาขาย่อย</t>
-  </si>
-  <si>
     <t xml:space="preserve">วันที่ใบกำกับภาษี</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t xml:space="preserve">ของลูกค้า/ผู้รับบริการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สาขาที่</t>
   </si>
   <si>
     <t xml:space="preserve">มูลค่าสินค้า</t>
@@ -95,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,13 +128,6 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -201,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,7 +209,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,19 +218,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -254,15 +233,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,11 +257,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,13 +348,13 @@
   </sheetPr>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.33"/>
@@ -426,128 +405,134 @@
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="H4" s="7" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="H5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+    </row>
+    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="G9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-    </row>
-    <row r="9" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14" t="s">
+      <c r="H9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="14" t="s">
+      <c r="I9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="19"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:H6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>

</xml_diff>

<commit_message>
[FIX] Input and Output report excel
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -188,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,10 +243,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -346,10 +342,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,14 +358,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -384,7 +381,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -399,9 +396,9 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -414,8 +411,8 @@
         <v>3</v>
       </c>
       <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
@@ -426,20 +423,21 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -452,7 +450,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="0"/>
-      <c r="K6" s="0"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
@@ -465,9 +463,9 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -491,15 +489,15 @@
         <v>15</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-    </row>
-    <row r="9" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -519,18 +517,18 @@
       <c r="I9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="17"/>
+      <c r="M9" s="16"/>
+      <c r="AMJ9" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
     <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="A8:A9"/>
@@ -539,7 +537,7 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[FIX] #1319 input tax not show cancel
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -344,8 +344,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[CHANGE] change name in menu report
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Input Tax Report" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Vat Report" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -344,8 +344,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[FIX] sequence input_report excel
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -49,13 +49,13 @@
     <t xml:space="preserve">ที่อยู่ :</t>
   </si>
   <si>
+    <t xml:space="preserve">ลำดับ</t>
+  </si>
+  <si>
     <t xml:space="preserve">วันที่ใบกำกับภาษี</t>
   </si>
   <si>
     <t xml:space="preserve">เลขที่อ้างอิง</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เลขที่ออกใหม่</t>
   </si>
   <si>
     <t xml:space="preserve">รายการ</t>
@@ -350,9 +350,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.24"/>

</xml_diff>